<commit_message>
Inclusão de número de tcc e dados de orientador
</commit_message>
<xml_diff>
--- a/AtaReuniao/TCC/DadosMalaDireta.xlsx
+++ b/AtaReuniao/TCC/DadosMalaDireta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trabalho\IFS\TCC\Leandro-2023.1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3513304B-B1F0-4011-9D68-4FF8B3067C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56C83A5-63E6-453F-A859-56BBA2CC3BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5AB74B04-0A8F-4E3C-B1E1-0102E974574E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Aluno</t>
   </si>
@@ -62,6 +62,9 @@
     <t>Coordenador</t>
   </si>
   <si>
+    <t>IFS TUTOR: UMA PROPOSTA DE CHATBOT PARA APOIO AOS ESTUDANTES DE NÍVEL SUPERIOR DO INSTITUTO FEDERAL DE SERGIPE</t>
+  </si>
+  <si>
     <t>HorarioFim</t>
   </si>
   <si>
@@ -110,25 +113,28 @@
     <t>Lagarto</t>
   </si>
   <si>
-    <t>[Aqui aparecerá o título do trabalho]</t>
-  </si>
-  <si>
-    <t>[Nome do aluno]</t>
-  </si>
-  <si>
-    <t>[Nome do co-orientador, caso exista]</t>
-  </si>
-  <si>
-    <t>[Nome do prof Examinador 2]</t>
-  </si>
-  <si>
-    <t>[Nome do prof Examinador 1]</t>
-  </si>
-  <si>
-    <t>[Nome do prof Orientador]</t>
-  </si>
-  <si>
-    <t>[Nome do coordenador]</t>
+    <t>NroTCC</t>
+  </si>
+  <si>
+    <t>SIAPE</t>
+  </si>
+  <si>
+    <t>Orientador ABC</t>
+  </si>
+  <si>
+    <t>Sou coorientador</t>
+  </si>
+  <si>
+    <t>Professor da banca 1</t>
+  </si>
+  <si>
+    <t>Professor da banca 2</t>
+  </si>
+  <si>
+    <t>Prof coordenador</t>
+  </si>
+  <si>
+    <t>Aluno que está defendendo</t>
   </si>
 </sst>
 </file>
@@ -512,35 +518,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C554E82-C001-436E-95A2-5AE59FFC107A}">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.88671875" customWidth="1"/>
     <col min="2" max="2" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="29.109375" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" customWidth="1"/>
-    <col min="6" max="6" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.88671875" customWidth="1"/>
+    <col min="3" max="3" width="9.88671875" customWidth="1"/>
+    <col min="4" max="5" width="13.88671875" customWidth="1"/>
+    <col min="6" max="6" width="29.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="8" max="8" width="3.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="3.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,146 +555,158 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="X1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1">
+        <v>12334443</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1">
+        <v>62</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2">
+        <v>45125</v>
+      </c>
+      <c r="H2" s="3">
+        <f>DAY(G2)</f>
+        <v>18</v>
+      </c>
+      <c r="I2" s="3" t="str">
+        <f>TEXT(G2,"mmmm")</f>
+        <v>julho</v>
+      </c>
+      <c r="J2" s="6">
+        <f>YEAR(G2)</f>
+        <v>2023</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="L2" s="1">
+        <f>HOUR(K2)</f>
+        <v>19</v>
+      </c>
+      <c r="M2" s="1">
+        <f>MINUTE(K2)</f>
+        <v>15</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="O2" s="1">
+        <f>HOUR(N2)</f>
+        <v>19</v>
+      </c>
+      <c r="P2" s="1">
+        <f>MINUTE(N2)</f>
+        <v>50</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="2">
-        <v>45125</v>
-      </c>
-      <c r="F2" s="3">
-        <f>DAY(E2)</f>
-        <v>18</v>
-      </c>
-      <c r="G2" s="3" t="str">
-        <f>TEXT(E2,"mmmm")</f>
-        <v>julho</v>
-      </c>
-      <c r="H2" s="6">
-        <f>YEAR(E2)</f>
-        <v>2023</v>
-      </c>
-      <c r="I2" s="4">
-        <v>0.80208333333333337</v>
-      </c>
-      <c r="J2" s="1">
-        <f>HOUR(I2)</f>
-        <v>19</v>
-      </c>
-      <c r="K2" s="1">
-        <f>MINUTE(I2)</f>
-        <v>15</v>
-      </c>
-      <c r="L2" s="5">
-        <v>0.82638888888888884</v>
-      </c>
-      <c r="M2" s="1">
-        <f>HOUR(L2)</f>
-        <v>19</v>
-      </c>
-      <c r="N2" s="1">
-        <f>MINUTE(L2)</f>
-        <v>50</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="R2" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>30</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U2" s="1">
         <v>10</v>
       </c>
-      <c r="V2" s="1" t="str">
-        <f>IF(U2&gt;=7,"APROVADO", "REPROVADO")</f>
+      <c r="U2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="W2" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="X2" s="1" t="str">
+        <f>IF(W2&gt;=7,"APROVADO", "REPROVADO")</f>
         <v>APROVADO</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>23</v>
+      <c r="Y2" s="1" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização da mala direta
</commit_message>
<xml_diff>
--- a/AtaReuniao/TCC/DadosMalaDireta.xlsx
+++ b/AtaReuniao/TCC/DadosMalaDireta.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trabalho\IFS\TCC\Leandro-2023.1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Trabalho\IFS\TCC\Alesson\Atas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B56C83A5-63E6-453F-A859-56BBA2CC3BDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32EDDB73-B677-43D1-8D0D-C432CFC7040C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5AB74B04-0A8F-4E3C-B1E1-0102E974574E}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Aluno</t>
   </si>
@@ -62,15 +65,9 @@
     <t>Coordenador</t>
   </si>
   <si>
-    <t>IFS TUTOR: UMA PROPOSTA DE CHATBOT PARA APOIO AOS ESTUDANTES DE NÍVEL SUPERIOR DO INSTITUTO FEDERAL DE SERGIPE</t>
-  </si>
-  <si>
     <t>HorarioFim</t>
   </si>
   <si>
-    <t>Instituto Federal de Educação, Ciência e Tecnologia de Sergipe</t>
-  </si>
-  <si>
     <t>HoraI</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>Curso</t>
   </si>
   <si>
-    <t>Bacharelado em Sistemas de Informação</t>
-  </si>
-  <si>
     <t>Situacao</t>
   </si>
   <si>
@@ -110,41 +104,24 @@
     <t>Cidade</t>
   </si>
   <si>
-    <t>Lagarto</t>
-  </si>
-  <si>
     <t>NroTCC</t>
   </si>
   <si>
     <t>SIAPE</t>
   </si>
   <si>
-    <t>Orientador ABC</t>
-  </si>
-  <si>
-    <t>Sou coorientador</t>
-  </si>
-  <si>
-    <t>Professor da banca 1</t>
-  </si>
-  <si>
-    <t>Professor da banca 2</t>
-  </si>
-  <si>
-    <t>Prof coordenador</t>
-  </si>
-  <si>
-    <t>Aluno que está defendendo</t>
+    <t>________</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="166" formatCode="?0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -183,7 +160,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -201,6 +178,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -221,10 +204,105 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="Dados básicos"/>
+      <sheetName val="Avaliador 1"/>
+      <sheetName val="Avaliador 2"/>
+      <sheetName val="Co-Orientador"/>
+      <sheetName val="Orientador"/>
+      <sheetName val="Resultado Final"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="4">
+          <cell r="B4" t="str">
+            <v>Nome completo do aluno</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="B5" t="str">
+            <v>Nome completo do orientador</v>
+          </cell>
+          <cell r="D5">
+            <v>987654</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="B6" t="str">
+            <v>Co-orinentador ou em branco</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="B7" t="str">
+            <v>Nome completo do avaliador 1</v>
+          </cell>
+          <cell r="D7" t="str">
+            <v>Instituto Federal de Educação, Ciência e Tecnologia de Sergipe</v>
+          </cell>
+        </row>
+        <row r="8">
+          <cell r="B8" t="str">
+            <v>Nome completo do avaliador 2</v>
+          </cell>
+          <cell r="D8" t="str">
+            <v>Instituto Federal de Educação, Ciência e Tecnologia de Sergipe</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="B9" t="str">
+            <v>Nome do coordenador de curso</v>
+          </cell>
+          <cell r="D9" t="str">
+            <v>Bacharelado em Sistemas de Informação</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="B10" t="str">
+            <v>Título do trabalho completo</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="B11">
+            <v>45314</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="B12">
+            <v>0.65833333333333333</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="B14" t="str">
+            <v>Lagarto</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5">
+        <row r="7">
+          <cell r="C7">
+            <v>8.7866666666666671</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office 2013 - 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -262,7 +340,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -368,7 +446,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -510,7 +588,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -520,8 +598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C554E82-C001-436E-95A2-5AE59FFC107A}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,6 +623,7 @@
     <col min="19" max="19" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="12.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.88671875" customWidth="1"/>
+    <col min="23" max="23" width="11.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -555,13 +634,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -573,101 +652,108 @@
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="P1" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:25" s="1" customFormat="1" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>27</v>
+      <c r="A2" s="1" t="str">
+        <f>'[1]Dados básicos'!$B$4</f>
+        <v>Nome completo do aluno</v>
+      </c>
+      <c r="B2" s="1" t="str">
+        <f>'[1]Dados básicos'!$B$5</f>
+        <v>Nome completo do orientador</v>
       </c>
       <c r="C2" s="1">
-        <v>12334443</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="1">
-        <v>62</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>8</v>
+        <f>'[1]Dados básicos'!$D$5</f>
+        <v>987654</v>
+      </c>
+      <c r="D2" s="1" t="str">
+        <f>IF(ISBLANK('[1]Dados básicos'!$B$6),"",'[1]Dados básicos'!$B$6)</f>
+        <v>Co-orinentador ou em branco</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="str">
+        <f>'[1]Dados básicos'!$B$10</f>
+        <v>Título do trabalho completo</v>
       </c>
       <c r="G2" s="2">
-        <v>45125</v>
+        <f>'[1]Dados básicos'!$B$11</f>
+        <v>45314</v>
       </c>
       <c r="H2" s="3">
         <f>DAY(G2)</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="I2" s="3" t="str">
         <f>TEXT(G2,"mmmm")</f>
-        <v>julho</v>
+        <v>janeiro</v>
       </c>
       <c r="J2" s="6">
         <f>YEAR(G2)</f>
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="K2" s="4">
-        <v>0.80208333333333337</v>
+        <f>'[1]Dados básicos'!$B$12</f>
+        <v>0.65833333333333333</v>
       </c>
       <c r="L2" s="1">
         <f>HOUR(K2)</f>
-        <v>19</v>
-      </c>
-      <c r="M2" s="1">
-        <f>MINUTE(K2)</f>
         <v>15</v>
+      </c>
+      <c r="M2" s="7" t="str">
+        <f>TEXT(MINUTE(K2),"00")</f>
+        <v>48</v>
       </c>
       <c r="N2" s="5">
         <v>0.82638888888888884</v>
@@ -676,37 +762,45 @@
         <f>HOUR(N2)</f>
         <v>19</v>
       </c>
-      <c r="P2" s="1">
-        <f>MINUTE(N2)</f>
+      <c r="P2" s="1" t="str">
+        <f>TEXT(MINUTE(N2), "00")</f>
         <v>50</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="W2" s="1">
-        <v>9.6999999999999993</v>
+      <c r="Q2" s="1" t="str">
+        <f>'[1]Dados básicos'!$B$7</f>
+        <v>Nome completo do avaliador 1</v>
+      </c>
+      <c r="R2" s="1" t="str">
+        <f>'[1]Dados básicos'!$D$7</f>
+        <v>Instituto Federal de Educação, Ciência e Tecnologia de Sergipe</v>
+      </c>
+      <c r="S2" s="1" t="str">
+        <f>'[1]Dados básicos'!$B$8</f>
+        <v>Nome completo do avaliador 2</v>
+      </c>
+      <c r="T2" s="1" t="str">
+        <f>'[1]Dados básicos'!$D$8</f>
+        <v>Instituto Federal de Educação, Ciência e Tecnologia de Sergipe</v>
+      </c>
+      <c r="U2" s="1" t="str">
+        <f>'[1]Dados básicos'!$B$9</f>
+        <v>Nome do coordenador de curso</v>
+      </c>
+      <c r="V2" s="1" t="str">
+        <f>'[1]Dados básicos'!$D$9</f>
+        <v>Bacharelado em Sistemas de Informação</v>
+      </c>
+      <c r="W2" s="8">
+        <f>'[1]Resultado Final'!$C$7</f>
+        <v>8.7866666666666671</v>
       </c>
       <c r="X2" s="1" t="str">
         <f>IF(W2&gt;=7,"APROVADO", "REPROVADO")</f>
         <v>APROVADO</v>
       </c>
-      <c r="Y2" s="1" t="s">
-        <v>24</v>
+      <c r="Y2" s="1" t="str">
+        <f>'[1]Dados básicos'!$B$14</f>
+        <v>Lagarto</v>
       </c>
     </row>
   </sheetData>

</xml_diff>